<commit_message>
Debugging the [BLANK] filler for the empty cells.
</commit_message>
<xml_diff>
--- a/src/main/resources/Key Records Sample.xlsx
+++ b/src/main/resources/Key Records Sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Computing\New Structure Folders\School_Management\Management Admin\Estates\Key Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwsco\IdeaProjects\KeyFinder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F683D-9FB7-4AB2-9AE0-A5313867A929}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fobs" sheetId="2" r:id="rId1"/>
@@ -18,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fobs!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$2:$D$69</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -428,7 +429,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -774,7 +775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -784,13 +785,13 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>122</v>
       </c>
@@ -798,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -806,7 +807,7 @@
         <v>89412</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -814,7 +815,7 @@
         <v>78920</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -822,7 +823,7 @@
         <v>55846</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -830,7 +831,7 @@
         <v>38945</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -838,7 +839,7 @@
         <v>10258</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -847,7 +848,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B7">
+  <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:B7">
       <sortCondition ref="A1:A7"/>
     </sortState>
@@ -858,8 +859,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:D69"/>
@@ -867,21 +868,21 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M23" sqref="M23"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -895,7 +896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>80</v>
       </c>
@@ -909,7 +910,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>80</v>
       </c>
@@ -923,7 +924,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>11254</v>
       </c>
@@ -934,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
@@ -945,7 +946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>125</v>
       </c>
@@ -956,7 +957,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>80</v>
       </c>
@@ -967,7 +968,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
@@ -978,7 +979,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -992,7 +993,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1022,7 +1023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>129</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>64</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>62</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>6499</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>39</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>41</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>34</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>35</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>40</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>87</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>42</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>38</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>8</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>5</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>128</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>126</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>126</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>73</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>77</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>49</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>127</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>127</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>127</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>127</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>75</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>23</v>
       </c>
@@ -1714,31 +1715,35 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D2">
+  <autoFilter ref="A2:D69" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
     <sortState ref="A3:D137">
       <sortCondition ref="D2"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1749,7 +1754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -1760,7 +1765,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -1771,7 +1776,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Starting to re-code the new load method.
</commit_message>
<xml_diff>
--- a/src/main/resources/Key Records Sample.xlsx
+++ b/src/main/resources/Key Records Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwsco\IdeaProjects\KeyFinder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F683D-9FB7-4AB2-9AE0-A5313867A929}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE933D6B-7B32-4D01-852A-B9F629CB8290}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fobs!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$2:$D$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$1:$D$68</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -473,10 +473,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -485,9 +484,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -788,14 +784,14 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -803,7 +799,7 @@
       <c r="A2" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>89412</v>
       </c>
     </row>
@@ -811,7 +807,7 @@
       <c r="A3" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>78920</v>
       </c>
     </row>
@@ -819,7 +815,7 @@
       <c r="A4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>55846</v>
       </c>
     </row>
@@ -827,7 +823,7 @@
       <c r="A5" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>38945</v>
       </c>
     </row>
@@ -835,7 +831,7 @@
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>10258</v>
       </c>
     </row>
@@ -843,7 +839,7 @@
       <c r="A7" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>88614</v>
       </c>
     </row>
@@ -860,867 +856,861 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M23" sqref="M23"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A2" s="2">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>11254</v>
       </c>
       <c r="C4" t="s">
         <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>11254</v>
+      <c r="A5" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>124</v>
+      <c r="A6" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>125</v>
+      <c r="A7" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>80</v>
+      <c r="A8" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>82</v>
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
       </c>
       <c r="D12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>108</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>59</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>103</v>
+      <c r="C16" t="s">
+        <v>108</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>103</v>
       </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
       <c r="D18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
-        <v>103</v>
+      <c r="C19" t="s">
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>32</v>
+      <c r="A20" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
+      <c r="A21" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C21" t="s">
         <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>28</v>
+      <c r="A22" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
         <v>108</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
+      <c r="A25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>57</v>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>56</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>53</v>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>54</v>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" t="s">
-        <v>103</v>
+      <c r="C31" t="s">
+        <v>108</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>17</v>
+      <c r="A32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>129</v>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>115</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>64</v>
+      <c r="A35" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>62</v>
+      <c r="A36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
+      <c r="A37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>6499</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
-        <v>6499</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>39</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>41</v>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>34</v>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>35</v>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>40</v>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>87</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" t="s">
-        <v>9</v>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>38</v>
+      <c r="A50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>8</v>
+      <c r="A51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>5</v>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>6</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1</v>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>128</v>
+      <c r="A55" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" t="s">
         <v>108</v>
-      </c>
-      <c r="D55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
       </c>
       <c r="D56" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>126</v>
+      <c r="A57" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C57" t="s">
         <v>108</v>
       </c>
       <c r="D57" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>73</v>
+      <c r="A58" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
+        <v>109</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D62" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B64" t="s">
         <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D64" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" t="s">
-        <v>61</v>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C65" t="s">
         <v>108</v>
       </c>
       <c r="D65" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>75</v>
+      <c r="A66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C67" t="s">
         <v>113</v>
       </c>
       <c r="D67" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>84</v>
+      <c r="A68" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C69" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D69" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="1">
-      <filters blank="1"/>
-    </filterColumn>
-    <sortState ref="A3:D137">
-      <sortCondition ref="D2"/>
+  <autoFilter ref="A1:D68" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState ref="A2:D136">
+      <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Testing and Optimisations for some of the methods.
</commit_message>
<xml_diff>
--- a/src/main/resources/Key Records Sample.xlsx
+++ b/src/main/resources/Key Records Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwsco\IdeaProjects\KeyFinder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE933D6B-7B32-4D01-852A-B9F629CB8290}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61AEF78-9605-4FDE-80F2-5B991E80D249}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fobs!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$1:$D$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Keys!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -864,7 +864,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M23" sqref="M23"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,7 +1568,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>77</v>
       </c>
@@ -1708,13 +1708,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D68" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:D136">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
starting to implement keywriter method to gui
</commit_message>
<xml_diff>
--- a/src/main/resources/Key Records Sample.xlsx
+++ b/src/main/resources/Key Records Sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwsco\IdeaProjects\KeyFinder\src\main\resources\"/>
     </mc:Choice>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="139">
   <si>
     <t>Fob Number</t>
   </si>
@@ -424,12 +424,37 @@
   </si>
   <si>
     <t>J Campbell</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2344</t>
+  </si>
+  <si>
+    <t>tamb</t>
+  </si>
+  <si>
+    <t>lewis</t>
+  </si>
+  <si>
+    <t>n533</t>
+  </si>
+  <si>
+    <t>4334</t>
+  </si>
+  <si>
+    <t>lle</t>
+  </si>
+  <si>
+    <t>n544</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -783,8 +808,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -859,7 +884,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -869,10 +894,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1705,6 +1730,328 @@
       </c>
       <c r="C68" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B73" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" t="s">
+        <v>131</v>
+      </c>
+      <c r="D75" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>131</v>
+      </c>
+      <c r="B76" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" t="s">
+        <v>131</v>
+      </c>
+      <c r="D76" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" t="s">
+        <v>131</v>
+      </c>
+      <c r="D77" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" t="s">
+        <v>131</v>
+      </c>
+      <c r="C78" t="s">
+        <v>131</v>
+      </c>
+      <c r="D78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>131</v>
+      </c>
+      <c r="B79" t="s">
+        <v>131</v>
+      </c>
+      <c r="C79" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>131</v>
+      </c>
+      <c r="B80" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" t="s">
+        <v>131</v>
+      </c>
+      <c r="D81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83" t="s">
+        <v>131</v>
+      </c>
+      <c r="D83" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" t="s">
+        <v>131</v>
+      </c>
+      <c r="C86" t="s">
+        <v>131</v>
+      </c>
+      <c r="D86" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" t="s">
+        <v>131</v>
+      </c>
+      <c r="D87" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" t="s">
+        <v>134</v>
+      </c>
+      <c r="D88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>131</v>
+      </c>
+      <c r="B89" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" t="s">
+        <v>131</v>
+      </c>
+      <c r="D89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>136</v>
+      </c>
+      <c r="B90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" t="s">
+        <v>134</v>
+      </c>
+      <c r="D90" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>131</v>
+      </c>
+      <c r="B91" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1727,9 +2074,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="1" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>